<commit_message>
fixed giftcards, added CreateAndRetrieveBooking script, added global variables
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manilacel/Library/CloudStorage/OneDrive-RoyalCaribbeanGroup/PMT/Git/RestructuredScript/pmt_katalon_local/Data Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k602p\Katalon Studio\PMT-GATEWAY-KATALON\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B463E074-5771-B94A-942F-33819A1E4EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFC4EF0-5B7F-4C48-9D08-26A5322B6826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ByCountryAndCurrency" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
   <si>
     <t>TCDescription</t>
   </si>
@@ -225,6 +225,20 @@
   <si>
     <t>xxx</t>
   </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>{
+  "validationMessage": "The cardNumber specified did not pass mod10 check or is invalid format."
+}</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t>errorCode": "PY-1501"</t>
+  </si>
 </sst>
 </file>
 
@@ -259,13 +273,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,16 +569,16 @@
       <selection activeCell="C4" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -584,7 +601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -607,7 +624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -630,7 +647,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -653,7 +670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -686,28 +703,28 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:I6"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -725,21 +742,21 @@
       <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -754,21 +771,21 @@
       <c r="G2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="H2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -783,21 +800,21 @@
       <c r="G3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -812,21 +829,21 @@
       <c r="G4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -841,21 +858,21 @@
       <c r="G5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -870,10 +887,10 @@
       <c r="G6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added PrevalidationsAndConf and other minor updates
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rccl-my.sharepoint.com/personal/charmainejaneelduayan_rcclapac_com/Documents/PMT/Git/RestructuredScript/TestingFolder/pmt_katalon_local/Data Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k602p\Katalon Studio\PMT-GATEWAY-KATALON\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{FBB975C2-4A0B-4BF1-8443-FAC250BF42CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87DDBE98-B768-2940-9792-4027BC481C4B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1694E977-BA10-4750-9953-3E721AFEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Validations_ByCtryOrCurr" sheetId="1" r:id="rId1"/>
-    <sheet name="GiftCards" sheetId="2" r:id="rId2"/>
-    <sheet name="cardTokenization_Encrypt" sheetId="3" r:id="rId3"/>
-    <sheet name="cardTokenization_Generate" sheetId="7" r:id="rId4"/>
-    <sheet name="ScheduledPayment_Get" sheetId="4" r:id="rId5"/>
-    <sheet name="ScheduledPayment_Add" sheetId="5" r:id="rId6"/>
-    <sheet name="ScheduledPayment_GetEligibility" sheetId="6" r:id="rId7"/>
+    <sheet name="GiftCards" sheetId="2" r:id="rId1"/>
+    <sheet name="cardTokenization_Encrypt" sheetId="3" r:id="rId2"/>
+    <sheet name="cardTokenization_Generate" sheetId="8" r:id="rId3"/>
+    <sheet name="ScheduledPayment_Get" sheetId="4" r:id="rId4"/>
+    <sheet name="ScheduledPayment_Add" sheetId="5" r:id="rId5"/>
+    <sheet name="ScheduledPayment_GetEligibility" sheetId="6" r:id="rId6"/>
+    <sheet name="Validations_Prevalidations&amp;Conf" sheetId="7" r:id="rId7"/>
+    <sheet name="Validations_ByCtryOrCurr" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="105">
   <si>
     <t>TCDescription</t>
   </si>
@@ -661,6 +662,38 @@
     <t>USA-Invalid currency</t>
   </si>
   <si>
+    <t>GET_ELIGIBILITY</t>
+  </si>
+  <si>
+    <t>Prevalidations&amp;Conf</t>
+  </si>
+  <si>
+    <t>Old booking</t>
+  </si>
+  <si>
+    <t>{
+  "errorCode": "PY-0701",
+  "errorMessage": "The request body did not pass input validation."
+}</t>
+  </si>
+  <si>
+    <t>{
+  "validationMessage": "The booking ID must be numeric."
+}</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>BookingId = existing booking + letter</t>
+  </si>
+  <si>
+    <t>259960A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
     <t>token</t>
   </si>
   <si>
@@ -734,10 +767,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1002,159 +1031,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE72FD-B2DC-F14E-AE74-63292B6A77A1}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -1212,7 +1110,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1241,7 +1139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1270,7 +1168,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1299,7 +1197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -1336,26 +1234,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D880AB4-1DE7-5946-BE4F-6F640D35FE1D}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1375,7 +1273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -1395,7 +1293,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1413,6 +1311,162 @@
       </c>
       <c r="F3" s="3" t="s">
         <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723A855F-829B-4B5D-8211-25823ECB6C26}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1421,154 +1475,342 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE581428-E8A0-8946-864F-922BD2565CB2}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B3E2DA-9933-4B77-A7B4-7C59CEE54D22}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
+      <c r="E2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>94</v>
+      <c r="E6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1577,350 +1819,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B3E2DA-9933-4B77-A7B4-7C59CEE54D22}">
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="26.83203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09718EF1-5D75-4972-9395-ACB737900D96}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -1928,20 +1826,20 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>45</v>
       </c>
@@ -1967,7 +1865,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -1993,7 +1891,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -2017,6 +1915,322 @@
       </c>
       <c r="H3" s="1" t="s">
         <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7BA175-0D7F-4BBD-B4FF-9DB63624C036}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2025,29 +2239,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7BA175-0D7F-4BBD-B4FF-9DB63624C036}">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE63EE0-2DBC-4407-96FB-89B2379A96F6}">
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>45</v>
       </c>
@@ -2079,12 +2293,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>38</v>
@@ -2108,15 +2322,15 @@
         <v>62</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>24</v>
@@ -2140,15 +2354,15 @@
         <v>67</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>29</v>
@@ -2172,15 +2386,15 @@
         <v>71</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>31</v>
@@ -2195,7 +2409,7 @@
         <v>69</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>71</v>
@@ -2204,15 +2418,15 @@
         <v>71</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
@@ -2236,15 +2450,15 @@
         <v>71</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>75</v>
@@ -2268,15 +2482,15 @@
         <v>71</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>78</v>
@@ -2285,7 +2499,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>69</v>
@@ -2300,15 +2514,15 @@
         <v>71</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>81</v>
@@ -2332,9 +2546,173 @@
         <v>71</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Payment Authorize Script
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rccl-my.sharepoint.com/personal/charmainejaneelduayan_rcclapac_com/Documents/PMT/Git/RestructuredScript/TestingFolder/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{1694E977-BA10-4750-9953-3E721AFEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8243BE92-D61C-674C-9149-E9CFE1A7C4EA}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:1_{1694E977-BA10-4750-9953-3E721AFEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29DF176A-9474-6A47-B586-05C93B0D7588}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="15840" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GiftCards" sheetId="2" r:id="rId1"/>
-    <sheet name="cardTokenization_Encrypt" sheetId="3" r:id="rId2"/>
-    <sheet name="cardTokenization_Generate" sheetId="8" r:id="rId3"/>
-    <sheet name="ScheduledPayment_Get" sheetId="4" r:id="rId4"/>
-    <sheet name="ScheduledPayment_Add" sheetId="5" r:id="rId5"/>
-    <sheet name="ScheduledPayment_GetEligibility" sheetId="6" r:id="rId6"/>
-    <sheet name="Validations_Prevalidations&amp;Conf" sheetId="7" r:id="rId7"/>
-    <sheet name="Validations_ByCtryOrCurr" sheetId="1" r:id="rId8"/>
-    <sheet name="Wallet_Add" sheetId="9" r:id="rId9"/>
-    <sheet name="Wallet_Replace" sheetId="10" r:id="rId10"/>
-    <sheet name="Wallet_Update" sheetId="11" r:id="rId11"/>
-    <sheet name="Wallet_Delete" sheetId="12" r:id="rId12"/>
+    <sheet name="Payment_Authorize" sheetId="13" r:id="rId2"/>
+    <sheet name="cardTokenization_Encrypt" sheetId="3" r:id="rId3"/>
+    <sheet name="cardTokenization_Generate" sheetId="8" r:id="rId4"/>
+    <sheet name="ScheduledPayment_Get" sheetId="4" r:id="rId5"/>
+    <sheet name="ScheduledPayment_Add" sheetId="5" r:id="rId6"/>
+    <sheet name="ScheduledPayment_GetEligibility" sheetId="6" r:id="rId7"/>
+    <sheet name="Validations_Prevalidations&amp;Conf" sheetId="7" r:id="rId8"/>
+    <sheet name="Validations_ByCtryOrCurr" sheetId="1" r:id="rId9"/>
+    <sheet name="Wallet_Add" sheetId="9" r:id="rId10"/>
+    <sheet name="Wallet_Replace" sheetId="10" r:id="rId11"/>
+    <sheet name="Wallet_Update" sheetId="11" r:id="rId12"/>
+    <sheet name="Wallet_Delete" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="155">
   <si>
     <t>TCDescription</t>
   </si>
@@ -747,6 +748,231 @@
   </si>
   <si>
     <t>Either card number or token is required</t>
+  </si>
+  <si>
+    <t>paymentChannel</t>
+  </si>
+  <si>
+    <t>ROYAL_WEB</t>
+  </si>
+  <si>
+    <t>orderId</t>
+  </si>
+  <si>
+    <t>7a4a85db-2fee-4026-b967-0e3aeff7e357</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>CRUISE_BOOKING</t>
+  </si>
+  <si>
+    <t>intent</t>
+  </si>
+  <si>
+    <t>AUTHORIZE</t>
+  </si>
+  <si>
+    <t>bookingId</t>
+  </si>
+  <si>
+    <t>passengerId</t>
+  </si>
+  <si>
+    <t>officeCode</t>
+  </si>
+  <si>
+    <t>countryCode</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>cvv</t>
+  </si>
+  <si>
+    <t>cardholder</t>
+  </si>
+  <si>
+    <t>addressOne</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zipCode</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>CARD</t>
+  </si>
+  <si>
+    <t>4387750107931111</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Obi-Wan</t>
+  </si>
+  <si>
+    <t>Obi-Wan's hut</t>
+  </si>
+  <si>
+    <t>Jundland Wastes</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
+    <t>33027</t>
+  </si>
+  <si>
+    <t>{
+  "header": {
+    "application": "celebritycriuses.com",
+    "brand": "${Brand}",
+    "domainId": "6",
+    "language": "en_US"
+  },
+  "countryCode": "USA",
+  "sailingInfo": {
+    "shipCode": "${ShipCode}",
+    "sailDate": "${SailDate}",
+    "packageCode": "${PackageId}",
+    "currencyCode": "USD"
+  },
+  "reservations": [
+    {
+      "cabin": {
+        "berthedCategoryCode": "${CategoryCode}",
+        "fareCode": "BESTRATE",
+        "pricedCategoryCode": "${CategoryCode}",
+        "waitListed": "false",
+        "accessible": "false",
+        "number": "${CabinNumber}"
+      },
+      "dining": [
+        {
+          "sitting": "O",
+          "sittingType": "OPEN",
+          "sittingInstance": "CEL SELECT"
+        }
+      ],
+      "gratuitiesPrepaid": "false",
+      "insurance": {
+        "code": "CRCR",
+        "optionIndicator": "false"
+      },
+      "fareQualifiers": {
+        "seniorReqd": "false",
+        "militaryReqd": "false",
+        "policeReqd": "false",
+        "fireFighterReqd": "false"
+      },
+      "guestDetails": [
+        {
+          "guestContact": {
+            "guestRefNumber": "0",
+            "personalInfo": {
+              "name": {
+                "title": "MS",
+                "firstName": "ESL One",
+                "lastName": "Tester"
+              },
+              "age": "55",
+              "birthDate": "1960-05-13",
+              "gender": "F",
+              "nationality": "USA"
+            },
+            "address": {
+              "address1": "addr1",
+              "city": "Miramar",
+              "stateCode": "FL",
+              "postalCode": "33029",
+              "countryName": "USA"
+            },
+            "email": "eslqa@rccl.com"
+          }
+        },
+        {
+          "guestContact": {
+            "guestRefNumber": "1",
+            "personalInfo": {
+              "name": {
+                "title": "MR",
+                "firstName": "ESL Two",
+                "lastName": "Tester"
+              },
+              "age": "55",
+              "birthDate": "1960-05-13",
+              "gender": "M",
+              "nationality": "USA"
+            },
+            "address": {
+              "address1": "addr1",
+              "city": "Miramar",
+              "stateCode": "NA",
+              "postalCode": "33029",
+              "countryName": "USA"
+            },
+            "email": "eslqa@rccl.com"
+          }
+        }
+      ],
+            "listOfCardPayments": {
+        "cardPayment": [
+          {
+            "cardType": "VA",
+            "cardToken": "4387751111111111",
+            "expireDate": "1230",
+            "amount": "100",
+            "currency": "USD",
+            "cvv": "123",
+            "extendPayments": "false",
+            "contact": {
+              "firstName": "PMT  QA",
+              "lastName": "Tester",
+              "address": {
+                "address1": "ADDRESS",
+                "city": "CITY",
+                "stateCode": "FLL",
+                "postalCode": "33019",
+                "countryCode": "USA",
+                "countryName": "USA"
+              }
+            }
+          }
+        ]
+      }
+    }
+  ],
+  "courtesyHold": "true"
+}</t>
+  </si>
+  <si>
+    <t>PassengerId</t>
+  </si>
+  <si>
+    <t>paymentType</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1314,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1288,6 +1514,164 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F02EF3-E80B-894D-87F6-2117279164FC}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="14.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="41.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="L5" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48459B2C-EE78-4646-A73A-554FA75BC79A}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -1414,7 +1798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22F0CD2-7E13-4747-A8F3-299BFC59F5E0}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -1572,12 +1956,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C96469-A5D6-3348-9B82-7D1CB15C18C4}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1731,6 +2115,275 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF1A0CB-9D4A-BD47-9E0E-F7867F60B0A1}">
+  <dimension ref="A1:AB5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="23" width="14.1640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="26.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="26.83203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="AB5" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D880AB4-1DE7-5946-BE4F-6F640D35FE1D}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1814,7 +2467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723A855F-829B-4B5D-8211-25823ECB6C26}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -1970,12 +2623,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B3E2DA-9933-4B77-A7B4-7C59CEE54D22}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2314,12 +2967,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09718EF1-5D75-4972-9395-ACB737900D96}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2378,7 +3031,7 @@
         <v>60</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>61</v>
+        <v>152</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>62</v>
@@ -2404,7 +3057,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>66</v>
+        <v>152</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>67</v>
@@ -2418,7 +3071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7BA175-0D7F-4BBD-B4FF-9DB63624C036}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -2734,7 +3387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE63EE0-2DBC-4407-96FB-89B2379A96F6}">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -3082,7 +3735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -3211,162 +3864,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F02EF3-E80B-894D-87F6-2117279164FC}">
-  <dimension ref="A1:L5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="14.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="41.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="L5" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Authorize Payment TC
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rccl-my.sharepoint.com/personal/charmainejaneelduayan_rcclapac_com/Documents/PMT/Git/RestructuredScript/TestingFolder/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{1694E977-BA10-4750-9953-3E721AFEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC23DECC-EAD3-D941-AC53-FE9C539FADC3}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{1694E977-BA10-4750-9953-3E721AFEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E59570C2-3754-124D-A607-8DD34AD4BA78}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GiftCards" sheetId="2" r:id="rId1"/>
-    <sheet name="Payment_Authorize" sheetId="13" r:id="rId2"/>
-    <sheet name="cardTokenization_Encrypt" sheetId="3" r:id="rId3"/>
-    <sheet name="cardTokenization_Generate" sheetId="8" r:id="rId4"/>
+    <sheet name="cardTokenization_Encrypt" sheetId="3" r:id="rId2"/>
+    <sheet name="cardTokenization_Generate" sheetId="8" r:id="rId3"/>
+    <sheet name="Payment_Authorize" sheetId="14" r:id="rId4"/>
     <sheet name="ScheduledPayment_Get" sheetId="4" r:id="rId5"/>
     <sheet name="ScheduledPayment_Add" sheetId="5" r:id="rId6"/>
     <sheet name="ScheduledPayment_GetEligibility" sheetId="6" r:id="rId7"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="157">
   <si>
     <t>TCDescription</t>
   </si>
@@ -973,6 +973,157 @@
   </si>
   <si>
     <t>paymentType</t>
+  </si>
+  <si>
+    <t>SELECT
+	SMBRND, 
+	SMSHIP, 
+	SUBSTR(ICSLMD.SMSDDT, 0, 0) || '20' || SUBSTR(ICSLMD.SMSDDT, 2, 2)|| '-' || SUBSTR(ICSLMD.SMSDDT, 4, 2)|| '-' || SUBSTR(ICSLMD.SMSDDT, 6, 2) AS SMSDDT, 
+	BHPKID,
+	CBCTCD, 
+	CBCBNO
+FROM 
+	ICSLMD 
+  	JOIN ICVCBD ON ICSLMD.SMSHIP = ICVCBD.CBSHIP AND ICSLMD.SMSDDT = ICVCBD.CBSDDT
+  	JOIN ICPKGD ON ICSLMD.SMITCD = ICPKGD.BHITCD
+  	JOIN DRDIDD ON ICSLMD.SMSHIP = DRDIDD.UFSHIP AND ICSLMD.SMSDDT = DRDIDD.UFSDDT
+ WHERE 
+ 	SMBRND = 'C'
+	AND SMSDDT &gt; Cast(Substr(Replace(Char(CURDATE() + 6 MONTH, ISO), '-', ''), 1) as Dec(8, 0))-19000000
+	AND ICVCBD.CBSTAT = 'AVL'
+	AND CBCBNO != 'GTY'
+	AND CBCABC = '2'
+	AND CBHNDA = ''
+	AND SMDSCD = 'O'
+	AND SMRSFG = 'Y'
+	AND SMINAF = 'Y'
+	AND SMSTAT != 'CX'
+	AND UFDTIM = 'OPEN'
+ORDER BY SMSDDT 
+	FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>{
+  "header": {
+    "application": "celebritycriuses.com",
+    "brand": "${Brand}",
+    "domainId": "6",
+    "language": "en_US"
+  },
+  "countryCode": "USA",
+  "sailingInfo": {
+    "shipCode": "${ShipCode}",
+    "sailDate": "${SailDate}",
+    "packageCode": "${PackageId}",
+    "currencyCode": "USD"
+  },
+  "reservations": [
+    {
+      "cabin": {
+        "berthedCategoryCode": "${CategoryCode}",
+        "fareCode": "BESTRATE",
+        "pricedCategoryCode": "${CategoryCode}",
+        "waitListed": "false",
+        "accessible": "false",
+        "number": "${CabinNumber}"
+      },
+      "dining": [
+        {
+          "sitting": "U",
+          "sittingType": "OPEN",
+          "sittingInstance": "CEL SELECT"
+        }
+      ],
+      "gratuitiesPrepaid": "false",
+      "insurance": {
+        "code": "CRCR",
+        "optionIndicator": "false"
+      },
+      "fareQualifiers": {
+        "seniorReqd": "false",
+        "militaryReqd": "false",
+        "policeReqd": "false",
+        "fireFighterReqd": "false"
+      },
+      "guestDetails": [
+        {
+          "guestContact": {
+            "guestRefNumber": "0",
+            "personalInfo": {
+              "name": {
+                "title": "MS",
+                "firstName": "ESL One",
+                "lastName": "Tester"
+              },
+              "age": "55",
+              "birthDate": "1960-05-13",
+              "gender": "F",
+              "nationality": "USA"
+            },
+            "address": {
+              "address1": "addr1",
+              "city": "Miramar",
+              "stateCode": "FL",
+              "postalCode": "33029",
+              "countryName": "USA"
+            },
+            "email": "eslqa@rccl.com"
+          }
+        },
+        {
+          "guestContact": {
+            "guestRefNumber": "1",
+            "personalInfo": {
+              "name": {
+                "title": "MR",
+                "firstName": "ESL Two",
+                "lastName": "Tester"
+              },
+              "age": "55",
+              "birthDate": "1960-05-13",
+              "gender": "M",
+              "nationality": "USA"
+            },
+            "address": {
+              "address1": "addr1",
+              "city": "Miramar",
+              "stateCode": "NA",
+              "postalCode": "33029",
+              "countryName": "USA"
+            },
+            "email": "eslqa@rccl.com"
+          }
+        }
+      ],
+            "listOfCardPayments": {
+        "cardPayment": [
+          {
+            "cardType": "VA",
+            "cardToken": "4387751111111111",
+            "expireDate": "1230",
+            "amount": "100",
+            "currency": "USD",
+            "cvv": "123",
+            "extendPayments": "false",
+            "contact": {
+              "firstName": "PMT  QA",
+              "lastName": "Tester",
+              "address": {
+                "address1": "ADDRESS",
+                "city": "CITY",
+                "stateCode": "FLL",
+                "postalCode": "33019",
+                "countryCode": "USA",
+                "countryName": "USA"
+              }
+            }
+          }
+        ]
+      }
+    }
+  ],
+  "courtesyHold": "true"
+}</t>
   </si>
 </sst>
 </file>
@@ -1314,7 +1465,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="A1:XFD1048576"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1326,7 +1477,7 @@
     <col min="5" max="5" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="61.1640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="21.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
@@ -2115,280 +2266,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF1A0CB-9D4A-BD47-9E0E-F7867F60B0A1}">
-  <dimension ref="A1:AB5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3:X11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="23" width="14.1640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="26.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.6640625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="26.83203125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.6640625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="AB4" s="3"/>
-    </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="AB5" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D880AB4-1DE7-5946-BE4F-6F640D35FE1D}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="A1:XFD1048576"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2467,12 +2349,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723A855F-829B-4B5D-8211-25823ECB6C26}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2623,12 +2505,299 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D43AD2-71CB-1D43-8E1D-EC2E182B29CC}">
+  <dimension ref="A1:AB3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="26.83203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B3E2DA-9933-4B77-A7B4-7C59CEE54D22}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2711,7 +2880,7 @@
         <v>61</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>63</v>
@@ -2746,7 +2915,7 @@
         <v>66</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>63</v>
@@ -2972,7 +3141,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3034,7 +3203,7 @@
         <v>152</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>63</v>
@@ -3060,7 +3229,7 @@
         <v>152</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>63</v>
@@ -3073,10 +3242,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7BA175-0D7F-4BBD-B4FF-9DB63624C036}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3152,7 +3321,7 @@
         <v>61</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>85</v>
@@ -3184,7 +3353,7 @@
         <v>66</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>86</v>
@@ -3380,6 +3549,11 @@
       </c>
       <c r="J9" s="3" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Script in Payment Authorization and Capture
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rccl-my.sharepoint.com/personal/charmainejaneelduayan_rcclapac_com/Documents/PMT/Git/RestructuredScript/TestingFolder/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{1694E977-BA10-4750-9953-3E721AFEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E59570C2-3754-124D-A607-8DD34AD4BA78}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:1_{1694E977-BA10-4750-9953-3E721AFEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E7E292E-D544-4344-A0B6-C33B2D59D2EA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GiftCards" sheetId="2" r:id="rId1"/>
     <sheet name="cardTokenization_Encrypt" sheetId="3" r:id="rId2"/>
     <sheet name="cardTokenization_Generate" sheetId="8" r:id="rId3"/>
-    <sheet name="Payment_Authorize" sheetId="14" r:id="rId4"/>
-    <sheet name="ScheduledPayment_Get" sheetId="4" r:id="rId5"/>
-    <sheet name="ScheduledPayment_Add" sheetId="5" r:id="rId6"/>
-    <sheet name="ScheduledPayment_GetEligibility" sheetId="6" r:id="rId7"/>
-    <sheet name="Validations_Prevalidations&amp;Conf" sheetId="7" r:id="rId8"/>
-    <sheet name="Validations_ByCtryOrCurr" sheetId="1" r:id="rId9"/>
-    <sheet name="Wallet_Add" sheetId="9" r:id="rId10"/>
-    <sheet name="Wallet_Replace" sheetId="10" r:id="rId11"/>
-    <sheet name="Wallet_Update" sheetId="11" r:id="rId12"/>
-    <sheet name="Wallet_Delete" sheetId="12" r:id="rId13"/>
+    <sheet name="Payment_Authorize" sheetId="15" r:id="rId4"/>
+    <sheet name="Payment_Capture" sheetId="14" r:id="rId5"/>
+    <sheet name="ScheduledPayment_Get" sheetId="4" r:id="rId6"/>
+    <sheet name="ScheduledPayment_Add" sheetId="5" r:id="rId7"/>
+    <sheet name="ScheduledPayment_GetEligibility" sheetId="6" r:id="rId8"/>
+    <sheet name="Validations_Prevalidations&amp;Conf" sheetId="7" r:id="rId9"/>
+    <sheet name="Validations_ByCtryOrCurr" sheetId="1" r:id="rId10"/>
+    <sheet name="Wallet_Add" sheetId="9" r:id="rId11"/>
+    <sheet name="Wallet_Replace" sheetId="10" r:id="rId12"/>
+    <sheet name="Wallet_Update" sheetId="11" r:id="rId13"/>
+    <sheet name="Wallet_Delete" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="158">
   <si>
     <t>TCDescription</t>
   </si>
@@ -846,129 +847,6 @@
     <t>33027</t>
   </si>
   <si>
-    <t>{
-  "header": {
-    "application": "celebritycriuses.com",
-    "brand": "${Brand}",
-    "domainId": "6",
-    "language": "en_US"
-  },
-  "countryCode": "USA",
-  "sailingInfo": {
-    "shipCode": "${ShipCode}",
-    "sailDate": "${SailDate}",
-    "packageCode": "${PackageId}",
-    "currencyCode": "USD"
-  },
-  "reservations": [
-    {
-      "cabin": {
-        "berthedCategoryCode": "${CategoryCode}",
-        "fareCode": "BESTRATE",
-        "pricedCategoryCode": "${CategoryCode}",
-        "waitListed": "false",
-        "accessible": "false",
-        "number": "${CabinNumber}"
-      },
-      "dining": [
-        {
-          "sitting": "O",
-          "sittingType": "OPEN",
-          "sittingInstance": "CEL SELECT"
-        }
-      ],
-      "gratuitiesPrepaid": "false",
-      "insurance": {
-        "code": "CRCR",
-        "optionIndicator": "false"
-      },
-      "fareQualifiers": {
-        "seniorReqd": "false",
-        "militaryReqd": "false",
-        "policeReqd": "false",
-        "fireFighterReqd": "false"
-      },
-      "guestDetails": [
-        {
-          "guestContact": {
-            "guestRefNumber": "0",
-            "personalInfo": {
-              "name": {
-                "title": "MS",
-                "firstName": "ESL One",
-                "lastName": "Tester"
-              },
-              "age": "55",
-              "birthDate": "1960-05-13",
-              "gender": "F",
-              "nationality": "USA"
-            },
-            "address": {
-              "address1": "addr1",
-              "city": "Miramar",
-              "stateCode": "FL",
-              "postalCode": "33029",
-              "countryName": "USA"
-            },
-            "email": "eslqa@rccl.com"
-          }
-        },
-        {
-          "guestContact": {
-            "guestRefNumber": "1",
-            "personalInfo": {
-              "name": {
-                "title": "MR",
-                "firstName": "ESL Two",
-                "lastName": "Tester"
-              },
-              "age": "55",
-              "birthDate": "1960-05-13",
-              "gender": "M",
-              "nationality": "USA"
-            },
-            "address": {
-              "address1": "addr1",
-              "city": "Miramar",
-              "stateCode": "NA",
-              "postalCode": "33029",
-              "countryName": "USA"
-            },
-            "email": "eslqa@rccl.com"
-          }
-        }
-      ],
-            "listOfCardPayments": {
-        "cardPayment": [
-          {
-            "cardType": "VA",
-            "cardToken": "4387751111111111",
-            "expireDate": "1230",
-            "amount": "100",
-            "currency": "USD",
-            "cvv": "123",
-            "extendPayments": "false",
-            "contact": {
-              "firstName": "PMT  QA",
-              "lastName": "Tester",
-              "address": {
-                "address1": "ADDRESS",
-                "city": "CITY",
-                "stateCode": "FLL",
-                "postalCode": "33019",
-                "countryCode": "USA",
-                "countryName": "USA"
-              }
-            }
-          }
-        ]
-      }
-    }
-  ],
-  "courtesyHold": "true"
-}</t>
-  </si>
-  <si>
     <t>PassengerId</t>
   </si>
   <si>
@@ -1001,6 +879,9 @@
 	AND UFDTIM = 'OPEN'
 ORDER BY SMSDDT 
 	FETCH FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>amount</t>
   </si>
   <si>
     <t>{
@@ -1052,7 +933,7 @@
             "personalInfo": {
               "name": {
                 "title": "MS",
-                "firstName": "ESL One",
+                "firstName": "PMT One",
                 "lastName": "Tester"
               },
               "age": "55",
@@ -1067,7 +948,7 @@
               "postalCode": "33029",
               "countryName": "USA"
             },
-            "email": "eslqa@rccl.com"
+            "email": "pmtqa@rccl.com"
           }
         },
         {
@@ -1076,7 +957,7 @@
             "personalInfo": {
               "name": {
                 "title": "MR",
-                "firstName": "ESL Two",
+                "firstName": "PMT Two",
                 "lastName": "Tester"
               },
               "age": "55",
@@ -1091,7 +972,7 @@
               "postalCode": "33029",
               "countryName": "USA"
             },
-            "email": "eslqa@rccl.com"
+            "email": "pmtqa@rccl.com"
           }
         }
       ],
@@ -1124,6 +1005,9 @@
   ],
   "courtesyHold": "true"
 }</t>
+  </si>
+  <si>
+    <t>CAPTURED</t>
   </si>
 </sst>
 </file>
@@ -1665,11 +1549,142 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F02EF3-E80B-894D-87F6-2117279164FC}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="A1:XFD1048576"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1822,7 +1837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48459B2C-EE78-4646-A73A-554FA75BC79A}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -1949,7 +1964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22F0CD2-7E13-4747-A8F3-299BFC59F5E0}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -2107,7 +2122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C96469-A5D6-3348-9B82-7D1CB15C18C4}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -2353,7 +2368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723A855F-829B-4B5D-8211-25823ECB6C26}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -2506,11 +2521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D43AD2-71CB-1D43-8E1D-EC2E182B29CC}">
-  <dimension ref="A1:AB3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0359A5F1-241A-D64B-BCC9-E10E2CDE789F}">
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2529,7 +2544,7 @@
     <col min="12" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2570,7 +2585,7 @@
         <v>133</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>103</v>
@@ -2599,23 +2614,20 @@
       <c r="W1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="X1" s="5" t="s">
-        <v>50</v>
+      <c r="X1" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z1" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="AA1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -2641,7 +2653,7 @@
         <v>51</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>140</v>
@@ -2686,22 +2698,19 @@
         <v>151</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA2" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -2727,7 +2736,7 @@
         <v>51</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>140</v>
@@ -2772,18 +2781,15 @@
         <v>151</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA3" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2793,11 +2799,78 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D43AD2-71CB-1D43-8E1D-EC2E182B29CC}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B3E2DA-9933-4B77-A7B4-7C59CEE54D22}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2877,10 +2950,10 @@
         <v>60</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>63</v>
@@ -2912,10 +2985,10 @@
         <v>65</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>63</v>
@@ -3136,12 +3209,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09718EF1-5D75-4972-9395-ACB737900D96}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3200,10 +3273,10 @@
         <v>60</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>63</v>
@@ -3226,10 +3299,10 @@
         <v>65</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>63</v>
@@ -3240,12 +3313,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7BA175-0D7F-4BBD-B4FF-9DB63624C036}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3318,10 +3391,10 @@
         <v>51</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>85</v>
@@ -3350,10 +3423,10 @@
         <v>51</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>86</v>
@@ -3561,7 +3634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE63EE0-2DBC-4407-96FB-89B2379A96F6}">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -3907,135 +3980,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes in GetEligibility and Add Script ConfirmWithRequest
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rccl-my.sharepoint.com/personal/charmainejaneelduayan_rcclapac_com/Documents/PMT/Git/RestructuredScript/TestingFolder/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:1_{1694E977-BA10-4750-9953-3E721AFEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E7E292E-D544-4344-A0B6-C33B2D59D2EA}"/>
+  <xr:revisionPtr revIDLastSave="305" documentId="13_ncr:1_{1694E977-BA10-4750-9953-3E721AFEAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57B921FC-0675-B047-9482-97CD4A3DAB90}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GiftCards" sheetId="2" r:id="rId1"/>
@@ -18,27 +18,39 @@
     <sheet name="cardTokenization_Generate" sheetId="8" r:id="rId3"/>
     <sheet name="Payment_Authorize" sheetId="15" r:id="rId4"/>
     <sheet name="Payment_Capture" sheetId="14" r:id="rId5"/>
-    <sheet name="ScheduledPayment_Get" sheetId="4" r:id="rId6"/>
-    <sheet name="ScheduledPayment_Add" sheetId="5" r:id="rId7"/>
-    <sheet name="ScheduledPayment_GetEligibility" sheetId="6" r:id="rId8"/>
-    <sheet name="Validations_Prevalidations&amp;Conf" sheetId="7" r:id="rId9"/>
-    <sheet name="Validations_ByCtryOrCurr" sheetId="1" r:id="rId10"/>
-    <sheet name="Wallet_Add" sheetId="9" r:id="rId11"/>
-    <sheet name="Wallet_Replace" sheetId="10" r:id="rId12"/>
-    <sheet name="Wallet_Update" sheetId="11" r:id="rId13"/>
-    <sheet name="Wallet_Delete" sheetId="12" r:id="rId14"/>
+    <sheet name="ScheduledPayment_GetEligibility" sheetId="17" r:id="rId6"/>
+    <sheet name="ScheduledPayment_ConfirmWithReq" sheetId="16" r:id="rId7"/>
+    <sheet name="ScheduledPayment_Get" sheetId="4" r:id="rId8"/>
+    <sheet name="ScheduledPayment_Add" sheetId="5" r:id="rId9"/>
+    <sheet name="Validations_Prevalidations&amp;Conf" sheetId="7" r:id="rId10"/>
+    <sheet name="Validations_ByCtryOrCurr" sheetId="1" r:id="rId11"/>
+    <sheet name="Wallet_Add" sheetId="9" r:id="rId12"/>
+    <sheet name="Wallet_Replace" sheetId="10" r:id="rId13"/>
+    <sheet name="Wallet_Update" sheetId="11" r:id="rId14"/>
+    <sheet name="Wallet_Delete" sheetId="12" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="170">
   <si>
     <t>TCDescription</t>
   </si>
@@ -647,9 +659,6 @@
     <t>"isEligible": true,</t>
   </si>
   <si>
-    <t>You must enter a valid booking ID having numeric string between 1 and 9999999, inclusive.</t>
-  </si>
-  <si>
     <t>Validations</t>
   </si>
   <si>
@@ -666,9 +675,6 @@
   </si>
   <si>
     <t>USA-Invalid currency</t>
-  </si>
-  <si>
-    <t>GET_ELIGIBILITY</t>
   </si>
   <si>
     <t>Prevalidations&amp;Conf</t>
@@ -1008,6 +1014,48 @@
   </si>
   <si>
     <t>CAPTURED</t>
+  </si>
+  <si>
+    <t>addressTwo</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>scheduledDate</t>
+  </si>
+  <si>
+    <t>20240704</t>
+  </si>
+  <si>
+    <t>100.25</t>
+  </si>
+  <si>
+    <t>totalAmount</t>
+  </si>
+  <si>
+    <t>50.25</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>passengerId1</t>
+  </si>
+  <si>
+    <t>passengerId2</t>
+  </si>
+  <si>
+    <t>amount1</t>
+  </si>
+  <si>
+    <t>amount2</t>
+  </si>
+  <si>
+    <t>isEligible</t>
+  </si>
+  <si>
+    <t>"status": 200</t>
   </si>
 </sst>
 </file>
@@ -1549,6 +1597,354 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE63EE0-2DBC-4407-96FB-89B2379A96F6}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -1598,10 +1994,10 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>38</v>
@@ -1610,7 +2006,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
@@ -1619,15 +2015,15 @@
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>24</v>
@@ -1636,7 +2032,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3</v>
@@ -1645,15 +2041,15 @@
         <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>29</v>
@@ -1662,7 +2058,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>3</v>
@@ -1679,7 +2075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F02EF3-E80B-894D-87F6-2117279164FC}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -1713,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -1725,13 +2121,13 @@
         <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
@@ -1751,7 +2147,7 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
@@ -1763,19 +2159,19 @@
         <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1786,13 +2182,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>18</v>
@@ -1801,19 +2197,19 @@
         <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1837,7 +2233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48459B2C-EE78-4646-A73A-554FA75BC79A}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -1872,10 +2268,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
@@ -1887,10 +2283,10 @@
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
@@ -1910,13 +2306,13 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>18</v>
@@ -1925,16 +2321,16 @@
         <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1964,7 +2360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22F0CD2-7E13-4747-A8F3-299BFC59F5E0}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -1998,7 +2394,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -2010,13 +2406,13 @@
         <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
@@ -2036,7 +2432,7 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
@@ -2048,19 +2444,19 @@
         <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2071,13 +2467,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>18</v>
@@ -2086,19 +2482,19 @@
         <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2122,7 +2518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C96469-A5D6-3348-9B82-7D1CB15C18C4}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -2156,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -2168,13 +2564,13 @@
         <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
@@ -2194,7 +2590,7 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
@@ -2206,19 +2602,19 @@
         <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2229,13 +2625,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>18</v>
@@ -2244,19 +2640,19 @@
         <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2431,10 +2827,10 @@
         <v>19</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2457,10 +2853,10 @@
         <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2486,7 +2882,7 @@
         <v>33</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2512,7 +2908,7 @@
         <v>33</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2522,15 +2918,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0359A5F1-241A-D64B-BCC9-E10E2CDE789F}">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" style="3" customWidth="1"/>
@@ -2544,75 +2940,75 @@
     <col min="12" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:28" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>53</v>
@@ -2620,14 +3016,15 @@
       <c r="Y1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB1" s="4"/>
+    </row>
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -2638,25 +3035,25 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>51</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>3</v>
@@ -2665,52 +3062,52 @@
         <v>4</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="X2" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -2721,25 +3118,25 @@
         <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>51</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>3</v>
@@ -2748,49 +3145,49 @@
         <v>4</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="X3" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2802,8 +3199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D43AD2-71CB-1D43-8E1D-EC2E182B29CC}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2825,7 +3222,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>54</v>
@@ -2848,16 +3245,16 @@
         <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2866,11 +3263,314 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A0C3C3-79E8-4C4C-A0A4-6463B25F2BAB}">
+  <dimension ref="A1:W3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="1" customWidth="1"/>
+    <col min="7" max="16" width="9.1640625" style="1"/>
+    <col min="17" max="17" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E73C8CAC-04FA-BA4D-9CDB-705D1EFFCB9E}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16" width="9.1640625" style="1"/>
+    <col min="17" max="17" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B3E2DA-9933-4B77-A7B4-7C59CEE54D22}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2950,10 +3650,10 @@
         <v>60</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>63</v>
@@ -2985,10 +3685,10 @@
         <v>65</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>63</v>
@@ -3209,12 +3909,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09718EF1-5D75-4972-9395-ACB737900D96}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3273,10 +3973,10 @@
         <v>60</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>63</v>
@@ -3299,682 +3999,13 @@
         <v>65</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7BA175-0D7F-4BBD-B4FF-9DB63624C036}">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H10" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE63EE0-2DBC-4407-96FB-89B2379A96F6}">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>